<commit_message>
Updated text on figures for circuit methodology document.
</commit_message>
<xml_diff>
--- a/docs/Figures/CircuitWorking.xlsx
+++ b/docs/Figures/CircuitWorking.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\engine\docs\Figures\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8ECE1969-901C-4DF4-A16E-0D727784D260}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-195" windowWidth="23700" windowHeight="12015" activeTab="1"/>
+    <workbookView xWindow="-60" yWindow="-195" windowWidth="23700" windowHeight="12015" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidationDataCircuitList" sheetId="4" r:id="rId1"/>
@@ -425,9 +431,6 @@
     <t>SwitchRCSINCurrent</t>
   </si>
   <si>
-    <t>BioGears Included</t>
-  </si>
-  <si>
     <t>Other Possible Extensions</t>
   </si>
   <si>
@@ -660,12 +663,15 @@
   </si>
   <si>
     <t>Intentionally failing adding voltage sources in parallel</t>
+  </si>
+  <si>
+    <t>Pulse Included</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1499,6 +1505,42 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1511,44 +1553,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1601,6 +1607,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1648,7 +1657,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1681,9 +1690,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1716,6 +1742,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1891,7 +1934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G100"/>
   <sheetViews>
@@ -1974,7 +2017,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>1</v>
@@ -1997,7 +2040,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>1</v>
@@ -2020,7 +2063,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G5" s="37" t="s">
         <v>1</v>
@@ -2043,7 +2086,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G6" s="37" t="s">
         <v>1</v>
@@ -2066,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G7" s="37" t="s">
         <v>1</v>
@@ -2089,7 +2132,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G8" s="37" t="s">
         <v>1</v>
@@ -2112,7 +2155,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G9" s="37" t="s">
         <v>1</v>
@@ -2135,7 +2178,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G10" s="37" t="s">
         <v>1</v>
@@ -2158,7 +2201,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G11" s="37" t="s">
         <v>1</v>
@@ -2181,7 +2224,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G12" s="37" t="s">
         <v>1</v>
@@ -2204,7 +2247,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G13" s="37" t="s">
         <v>1</v>
@@ -2227,7 +2270,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G14" s="37" t="s">
         <v>1</v>
@@ -2250,7 +2293,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G15" s="37" t="s">
         <v>1</v>
@@ -2273,7 +2316,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G16" s="37" t="s">
         <v>1</v>
@@ -2296,7 +2339,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G17" s="37" t="s">
         <v>1</v>
@@ -2319,7 +2362,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G18" s="37" t="s">
         <v>1</v>
@@ -2342,7 +2385,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G19" s="37" t="s">
         <v>1</v>
@@ -2365,7 +2408,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G20" s="37" t="s">
         <v>1</v>
@@ -2388,7 +2431,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G21" s="37" t="s">
         <v>1</v>
@@ -2411,7 +2454,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G22" s="37" t="s">
         <v>1</v>
@@ -2434,7 +2477,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G23" s="37" t="s">
         <v>1</v>
@@ -2457,7 +2500,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G24" s="37" t="s">
         <v>1</v>
@@ -2480,7 +2523,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G25" s="37" t="s">
         <v>1</v>
@@ -2503,7 +2546,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G26" s="37" t="s">
         <v>1</v>
@@ -2526,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G27" s="37" t="s">
         <v>1</v>
@@ -2549,7 +2592,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G28" s="37" t="s">
         <v>1</v>
@@ -2572,7 +2615,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G29" s="37" t="s">
         <v>1</v>
@@ -2595,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G30" s="37" t="s">
         <v>1</v>
@@ -2612,13 +2655,13 @@
         <v>1</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E31" s="37" t="s">
         <v>1</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G31" s="37" t="s">
         <v>1</v>
@@ -2635,13 +2678,13 @@
         <v>1</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E32" s="37" t="s">
         <v>1</v>
       </c>
       <c r="F32" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G32" s="37" t="s">
         <v>1</v>
@@ -2658,13 +2701,13 @@
         <v>1</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E33" s="37" t="s">
         <v>1</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G33" s="37" t="s">
         <v>1</v>
@@ -2687,7 +2730,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G34" s="37" t="s">
         <v>1</v>
@@ -2710,7 +2753,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G35" s="37" t="s">
         <v>1</v>
@@ -2733,7 +2776,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G36" s="37" t="s">
         <v>1</v>
@@ -2756,7 +2799,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G37" s="37" t="s">
         <v>1</v>
@@ -2779,7 +2822,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G38" s="37" t="s">
         <v>1</v>
@@ -2802,13 +2845,13 @@
         <v>1</v>
       </c>
       <c r="F39" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G39" s="37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
         <v>1</v>
       </c>
@@ -2825,13 +2868,13 @@
         <v>1</v>
       </c>
       <c r="F40" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G40" s="37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="37" t="s">
         <v>1</v>
       </c>
@@ -2848,13 +2891,13 @@
         <v>1</v>
       </c>
       <c r="F41" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G41" s="37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="s">
         <v>1</v>
       </c>
@@ -2871,13 +2914,13 @@
         <v>1</v>
       </c>
       <c r="F42" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G42" s="37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="37" t="s">
         <v>1</v>
       </c>
@@ -2894,13 +2937,13 @@
         <v>1</v>
       </c>
       <c r="F43" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G43" s="37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="37" t="s">
         <v>1</v>
       </c>
@@ -2917,13 +2960,13 @@
         <v>1</v>
       </c>
       <c r="F44" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G44" s="37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="37" t="s">
         <v>1</v>
       </c>
@@ -2940,13 +2983,13 @@
         <v>1</v>
       </c>
       <c r="F45" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G45" s="37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="37" t="s">
         <v>1</v>
       </c>
@@ -2963,13 +3006,13 @@
         <v>1</v>
       </c>
       <c r="F46" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G46" s="37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="37" t="s">
         <v>1</v>
       </c>
@@ -2986,13 +3029,13 @@
         <v>1</v>
       </c>
       <c r="F47" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G47" s="37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="37" t="s">
         <v>1</v>
       </c>
@@ -3009,7 +3052,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G48" s="37" t="s">
         <v>1</v>
@@ -3032,7 +3075,7 @@
         <v>1</v>
       </c>
       <c r="F49" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G49" s="37" t="s">
         <v>1</v>
@@ -3055,7 +3098,7 @@
         <v>1</v>
       </c>
       <c r="F50" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G50" s="37" t="s">
         <v>1</v>
@@ -3078,7 +3121,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G51" s="37" t="s">
         <v>1</v>
@@ -3101,7 +3144,7 @@
         <v>1</v>
       </c>
       <c r="F52" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G52" s="37" t="s">
         <v>1</v>
@@ -3124,7 +3167,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G53" s="37" t="s">
         <v>1</v>
@@ -3147,7 +3190,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G54" s="37" t="s">
         <v>1</v>
@@ -3170,7 +3213,7 @@
         <v>1</v>
       </c>
       <c r="F55" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G55" s="37" t="s">
         <v>1</v>
@@ -3193,7 +3236,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G56" s="37" t="s">
         <v>1</v>
@@ -3216,7 +3259,7 @@
         <v>1</v>
       </c>
       <c r="F57" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G57" s="37" t="s">
         <v>1</v>
@@ -3239,7 +3282,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G58" s="37" t="s">
         <v>1</v>
@@ -3262,7 +3305,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G59" s="37" t="s">
         <v>1</v>
@@ -3285,7 +3328,7 @@
         <v>1</v>
       </c>
       <c r="F60" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G60" s="37" t="s">
         <v>1</v>
@@ -3308,7 +3351,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G61" s="37" t="s">
         <v>1</v>
@@ -3331,7 +3374,7 @@
         <v>1</v>
       </c>
       <c r="F62" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G62" s="37" t="s">
         <v>1</v>
@@ -3354,7 +3397,7 @@
         <v>1</v>
       </c>
       <c r="F63" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G63" s="37" t="s">
         <v>1</v>
@@ -3377,7 +3420,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G64" s="37" t="s">
         <v>1</v>
@@ -3400,7 +3443,7 @@
         <v>1</v>
       </c>
       <c r="F65" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G65" s="37" t="s">
         <v>1</v>
@@ -3423,7 +3466,7 @@
         <v>1</v>
       </c>
       <c r="F66" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G66" s="37" t="s">
         <v>1</v>
@@ -3446,7 +3489,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G67" s="37" t="s">
         <v>1</v>
@@ -3469,7 +3512,7 @@
         <v>1</v>
       </c>
       <c r="F68" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G68" s="37" t="s">
         <v>1</v>
@@ -3492,7 +3535,7 @@
         <v>1</v>
       </c>
       <c r="F69" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G69" s="37" t="s">
         <v>1</v>
@@ -3515,7 +3558,7 @@
         <v>1</v>
       </c>
       <c r="F70" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G70" s="37" t="s">
         <v>1</v>
@@ -3538,7 +3581,7 @@
         <v>1</v>
       </c>
       <c r="F71" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G71" s="37" t="s">
         <v>1</v>
@@ -3561,7 +3604,7 @@
         <v>1</v>
       </c>
       <c r="F72" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G72" s="37" t="s">
         <v>1</v>
@@ -3584,7 +3627,7 @@
         <v>1</v>
       </c>
       <c r="F73" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G73" s="37" t="s">
         <v>1</v>
@@ -3607,7 +3650,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G74" s="37" t="s">
         <v>1</v>
@@ -3630,7 +3673,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G75" s="37" t="s">
         <v>1</v>
@@ -3653,7 +3696,7 @@
         <v>1</v>
       </c>
       <c r="F76" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G76" s="37" t="s">
         <v>1</v>
@@ -3676,7 +3719,7 @@
         <v>1</v>
       </c>
       <c r="F77" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G77" s="37" t="s">
         <v>1</v>
@@ -3699,7 +3742,7 @@
         <v>1</v>
       </c>
       <c r="F78" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G78" s="37" t="s">
         <v>1</v>
@@ -3722,7 +3765,7 @@
         <v>1</v>
       </c>
       <c r="F79" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G79" s="37" t="s">
         <v>1</v>
@@ -3745,7 +3788,7 @@
         <v>1</v>
       </c>
       <c r="F80" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G80" s="37" t="s">
         <v>1</v>
@@ -3768,7 +3811,7 @@
         <v>1</v>
       </c>
       <c r="F81" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G81" s="37" t="s">
         <v>1</v>
@@ -3791,7 +3834,7 @@
         <v>1</v>
       </c>
       <c r="F82" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G82" s="37" t="s">
         <v>1</v>
@@ -3814,7 +3857,7 @@
         <v>1</v>
       </c>
       <c r="F83" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G83" s="37" t="s">
         <v>1</v>
@@ -3837,7 +3880,7 @@
         <v>1</v>
       </c>
       <c r="F84" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G84" s="37" t="s">
         <v>1</v>
@@ -3860,7 +3903,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G85" s="37" t="s">
         <v>1</v>
@@ -3883,7 +3926,7 @@
         <v>1</v>
       </c>
       <c r="F86" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G86" s="37" t="s">
         <v>1</v>
@@ -3906,7 +3949,7 @@
         <v>1</v>
       </c>
       <c r="F87" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G87" s="37" t="s">
         <v>1</v>
@@ -3929,7 +3972,7 @@
         <v>1</v>
       </c>
       <c r="F88" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G88" s="37" t="s">
         <v>1</v>
@@ -3952,7 +3995,7 @@
         <v>1</v>
       </c>
       <c r="F89" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G89" s="37" t="s">
         <v>1</v>
@@ -3975,7 +4018,7 @@
         <v>1</v>
       </c>
       <c r="F90" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G90" s="37" t="s">
         <v>1</v>
@@ -3998,7 +4041,7 @@
         <v>1</v>
       </c>
       <c r="F91" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G91" s="37" t="s">
         <v>1</v>
@@ -4021,7 +4064,7 @@
         <v>1</v>
       </c>
       <c r="F92" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G92" s="37" t="s">
         <v>1</v>
@@ -4044,7 +4087,7 @@
         <v>1</v>
       </c>
       <c r="F93" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G93" s="37" t="s">
         <v>1</v>
@@ -4067,7 +4110,7 @@
         <v>1</v>
       </c>
       <c r="F94" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G94" s="37" t="s">
         <v>1</v>
@@ -4090,7 +4133,7 @@
         <v>1</v>
       </c>
       <c r="F95" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G95" s="37" t="s">
         <v>1</v>
@@ -4113,7 +4156,7 @@
         <v>1</v>
       </c>
       <c r="F96" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G96" s="37" t="s">
         <v>1</v>
@@ -4136,7 +4179,7 @@
         <v>1</v>
       </c>
       <c r="F97" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G97" s="37" t="s">
         <v>1</v>
@@ -4159,7 +4202,7 @@
         <v>1</v>
       </c>
       <c r="F98" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G98" s="37" t="s">
         <v>1</v>
@@ -4182,7 +4225,7 @@
         <v>1</v>
       </c>
       <c r="F99" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G99" s="37" t="s">
         <v>1</v>
@@ -4205,7 +4248,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G100" s="37" t="s">
         <v>1</v>
@@ -4218,12 +4261,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="B1:K15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E2" sqref="E2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4237,335 +4280,335 @@
   <sheetData>
     <row r="1" spans="2:11" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="53" t="s">
+      <c r="B2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="38" t="s">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="40"/>
-    </row>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="51"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="K3" s="6" t="s">
+    </row>
+    <row r="4" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="53" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="41" t="s">
+      <c r="C4" s="54" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="D4" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="J4" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="K4" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="K4" s="13" t="s">
+    </row>
+    <row r="5" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="39"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="14" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="42"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="G5" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="H5" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="I5" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="K5" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="39"/>
+      <c r="C6" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="K5" s="19" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="45" t="s">
+      <c r="D6" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="E6" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="F6" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="H6" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="H6" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="K6" s="22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="40"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="K6" s="22" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="43"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="23" t="s">
+      <c r="E7" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="F7" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="G7" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="H7" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="I7" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="K7" s="28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="K7" s="28" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="47" t="s">
+      <c r="C8" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="D8" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="E8" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="F8" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="I8" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="J8" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="G8" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="I8" s="33" t="s">
+      <c r="K8" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="J8" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="K8" s="35" t="s">
+    </row>
+    <row r="9" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="39"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="14" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="42"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="14" t="s">
+      <c r="E9" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="F9" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="G9" s="16" t="s">
+      <c r="J9" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="39"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="G10" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="H9" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="42"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="14" t="s">
+      <c r="H10" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="I10" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="K10" s="22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="39"/>
+      <c r="C11" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="K10" s="22" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="42"/>
-      <c r="C11" s="45" t="s">
+      <c r="D11" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="F11" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="G11" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="H11" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="I11" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="K11" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="K11" s="19" t="s">
+    </row>
+    <row r="12" spans="2:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="40"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="23" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="43"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="23" t="s">
+      <c r="E12" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="F12" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="G12" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="H12" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="I12" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="K12" s="28" t="s">
         <v>205</v>
-      </c>
-      <c r="K12" s="28" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D14" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>207</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="B8:B12"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated circuit analogy table.
</commit_message>
<xml_diff>
--- a/docs/Figures/CircuitWorking.xlsx
+++ b/docs/Figures/CircuitWorking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\engine\docs\Figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\4x-Source\docs\Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8ECE1969-901C-4DF4-A16E-0D727784D260}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A093F377-7F56-44E3-B672-CA457A5BE2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-195" windowWidth="23700" windowHeight="12015" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10605" yWindow="6765" windowWidth="23370" windowHeight="21795" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidationDataCircuitList" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="216">
   <si>
     <t>Description</t>
   </si>
@@ -560,9 +560,6 @@
     <t>Resistance</t>
   </si>
   <si>
-    <t>Damping</t>
-  </si>
-  <si>
     <t>Clearance</t>
   </si>
   <si>
@@ -584,12 +581,6 @@
     <t>Inductance</t>
   </si>
   <si>
-    <t>Stiffness</t>
-  </si>
-  <si>
-    <t>Torsional Stiffness</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -666,6 +657,18 @@
   </si>
   <si>
     <t>Pulse Included</t>
+  </si>
+  <si>
+    <t>Damping Reciprocal</t>
+  </si>
+  <si>
+    <t>Stiffness Reciprocal</t>
+  </si>
+  <si>
+    <t>Torsional Stiffness Reciprocal</t>
+  </si>
+  <si>
+    <t>Rotary Damping Reciprocal</t>
   </si>
 </sst>
 </file>
@@ -1505,24 +1508,39 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1540,21 +1558,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2017,7 +2020,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>1</v>
@@ -2040,7 +2043,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>1</v>
@@ -2063,7 +2066,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G5" s="37" t="s">
         <v>1</v>
@@ -2086,7 +2089,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G6" s="37" t="s">
         <v>1</v>
@@ -2109,7 +2112,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G7" s="37" t="s">
         <v>1</v>
@@ -2132,7 +2135,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G8" s="37" t="s">
         <v>1</v>
@@ -2155,7 +2158,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G9" s="37" t="s">
         <v>1</v>
@@ -2178,7 +2181,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G10" s="37" t="s">
         <v>1</v>
@@ -2201,7 +2204,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G11" s="37" t="s">
         <v>1</v>
@@ -2224,7 +2227,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G12" s="37" t="s">
         <v>1</v>
@@ -2247,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G13" s="37" t="s">
         <v>1</v>
@@ -2270,7 +2273,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G14" s="37" t="s">
         <v>1</v>
@@ -2293,7 +2296,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G15" s="37" t="s">
         <v>1</v>
@@ -2316,7 +2319,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G16" s="37" t="s">
         <v>1</v>
@@ -2339,7 +2342,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G17" s="37" t="s">
         <v>1</v>
@@ -2362,7 +2365,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G18" s="37" t="s">
         <v>1</v>
@@ -2385,7 +2388,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G19" s="37" t="s">
         <v>1</v>
@@ -2408,7 +2411,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G20" s="37" t="s">
         <v>1</v>
@@ -2431,7 +2434,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G21" s="37" t="s">
         <v>1</v>
@@ -2454,7 +2457,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G22" s="37" t="s">
         <v>1</v>
@@ -2477,7 +2480,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G23" s="37" t="s">
         <v>1</v>
@@ -2500,7 +2503,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G24" s="37" t="s">
         <v>1</v>
@@ -2523,7 +2526,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G25" s="37" t="s">
         <v>1</v>
@@ -2546,7 +2549,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G26" s="37" t="s">
         <v>1</v>
@@ -2569,7 +2572,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G27" s="37" t="s">
         <v>1</v>
@@ -2592,7 +2595,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G28" s="37" t="s">
         <v>1</v>
@@ -2615,7 +2618,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G29" s="37" t="s">
         <v>1</v>
@@ -2638,7 +2641,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G30" s="37" t="s">
         <v>1</v>
@@ -2655,13 +2658,13 @@
         <v>1</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E31" s="37" t="s">
         <v>1</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G31" s="37" t="s">
         <v>1</v>
@@ -2678,13 +2681,13 @@
         <v>1</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E32" s="37" t="s">
         <v>1</v>
       </c>
       <c r="F32" s="37" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G32" s="37" t="s">
         <v>1</v>
@@ -2701,13 +2704,13 @@
         <v>1</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E33" s="37" t="s">
         <v>1</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G33" s="37" t="s">
         <v>1</v>
@@ -2730,7 +2733,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G34" s="37" t="s">
         <v>1</v>
@@ -2753,7 +2756,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G35" s="37" t="s">
         <v>1</v>
@@ -2776,7 +2779,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G36" s="37" t="s">
         <v>1</v>
@@ -2799,7 +2802,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G37" s="37" t="s">
         <v>1</v>
@@ -2822,7 +2825,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G38" s="37" t="s">
         <v>1</v>
@@ -2845,7 +2848,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G39" s="37" t="s">
         <v>1</v>
@@ -2868,7 +2871,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G40" s="37" t="s">
         <v>1</v>
@@ -2891,7 +2894,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G41" s="37" t="s">
         <v>1</v>
@@ -2914,7 +2917,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G42" s="37" t="s">
         <v>1</v>
@@ -2937,7 +2940,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G43" s="37" t="s">
         <v>1</v>
@@ -2960,7 +2963,7 @@
         <v>1</v>
       </c>
       <c r="F44" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G44" s="37" t="s">
         <v>1</v>
@@ -2983,7 +2986,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G45" s="37" t="s">
         <v>1</v>
@@ -3006,7 +3009,7 @@
         <v>1</v>
       </c>
       <c r="F46" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G46" s="37" t="s">
         <v>1</v>
@@ -3029,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="F47" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G47" s="37" t="s">
         <v>1</v>
@@ -3052,7 +3055,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G48" s="37" t="s">
         <v>1</v>
@@ -3075,7 +3078,7 @@
         <v>1</v>
       </c>
       <c r="F49" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G49" s="37" t="s">
         <v>1</v>
@@ -3098,7 +3101,7 @@
         <v>1</v>
       </c>
       <c r="F50" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G50" s="37" t="s">
         <v>1</v>
@@ -3121,7 +3124,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G51" s="37" t="s">
         <v>1</v>
@@ -3144,7 +3147,7 @@
         <v>1</v>
       </c>
       <c r="F52" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G52" s="37" t="s">
         <v>1</v>
@@ -3167,7 +3170,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G53" s="37" t="s">
         <v>1</v>
@@ -3190,7 +3193,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G54" s="37" t="s">
         <v>1</v>
@@ -3213,7 +3216,7 @@
         <v>1</v>
       </c>
       <c r="F55" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G55" s="37" t="s">
         <v>1</v>
@@ -3236,7 +3239,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G56" s="37" t="s">
         <v>1</v>
@@ -3259,7 +3262,7 @@
         <v>1</v>
       </c>
       <c r="F57" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G57" s="37" t="s">
         <v>1</v>
@@ -3282,7 +3285,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G58" s="37" t="s">
         <v>1</v>
@@ -3305,7 +3308,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G59" s="37" t="s">
         <v>1</v>
@@ -3328,7 +3331,7 @@
         <v>1</v>
       </c>
       <c r="F60" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G60" s="37" t="s">
         <v>1</v>
@@ -3351,7 +3354,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G61" s="37" t="s">
         <v>1</v>
@@ -3374,7 +3377,7 @@
         <v>1</v>
       </c>
       <c r="F62" s="37" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G62" s="37" t="s">
         <v>1</v>
@@ -3397,7 +3400,7 @@
         <v>1</v>
       </c>
       <c r="F63" s="37" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G63" s="37" t="s">
         <v>1</v>
@@ -3420,7 +3423,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="37" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G64" s="37" t="s">
         <v>1</v>
@@ -3443,7 +3446,7 @@
         <v>1</v>
       </c>
       <c r="F65" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G65" s="37" t="s">
         <v>1</v>
@@ -3466,7 +3469,7 @@
         <v>1</v>
       </c>
       <c r="F66" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G66" s="37" t="s">
         <v>1</v>
@@ -3489,7 +3492,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G67" s="37" t="s">
         <v>1</v>
@@ -3512,7 +3515,7 @@
         <v>1</v>
       </c>
       <c r="F68" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G68" s="37" t="s">
         <v>1</v>
@@ -3535,7 +3538,7 @@
         <v>1</v>
       </c>
       <c r="F69" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G69" s="37" t="s">
         <v>1</v>
@@ -3558,7 +3561,7 @@
         <v>1</v>
       </c>
       <c r="F70" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G70" s="37" t="s">
         <v>1</v>
@@ -3581,7 +3584,7 @@
         <v>1</v>
       </c>
       <c r="F71" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G71" s="37" t="s">
         <v>1</v>
@@ -3604,7 +3607,7 @@
         <v>1</v>
       </c>
       <c r="F72" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G72" s="37" t="s">
         <v>1</v>
@@ -3627,7 +3630,7 @@
         <v>1</v>
       </c>
       <c r="F73" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G73" s="37" t="s">
         <v>1</v>
@@ -3650,7 +3653,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G74" s="37" t="s">
         <v>1</v>
@@ -3673,7 +3676,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G75" s="37" t="s">
         <v>1</v>
@@ -3696,7 +3699,7 @@
         <v>1</v>
       </c>
       <c r="F76" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G76" s="37" t="s">
         <v>1</v>
@@ -3719,7 +3722,7 @@
         <v>1</v>
       </c>
       <c r="F77" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G77" s="37" t="s">
         <v>1</v>
@@ -3742,7 +3745,7 @@
         <v>1</v>
       </c>
       <c r="F78" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G78" s="37" t="s">
         <v>1</v>
@@ -3765,7 +3768,7 @@
         <v>1</v>
       </c>
       <c r="F79" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G79" s="37" t="s">
         <v>1</v>
@@ -3788,7 +3791,7 @@
         <v>1</v>
       </c>
       <c r="F80" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G80" s="37" t="s">
         <v>1</v>
@@ -3811,7 +3814,7 @@
         <v>1</v>
       </c>
       <c r="F81" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G81" s="37" t="s">
         <v>1</v>
@@ -3834,7 +3837,7 @@
         <v>1</v>
       </c>
       <c r="F82" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G82" s="37" t="s">
         <v>1</v>
@@ -3857,7 +3860,7 @@
         <v>1</v>
       </c>
       <c r="F83" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G83" s="37" t="s">
         <v>1</v>
@@ -3880,7 +3883,7 @@
         <v>1</v>
       </c>
       <c r="F84" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G84" s="37" t="s">
         <v>1</v>
@@ -3903,7 +3906,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G85" s="37" t="s">
         <v>1</v>
@@ -3926,7 +3929,7 @@
         <v>1</v>
       </c>
       <c r="F86" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G86" s="37" t="s">
         <v>1</v>
@@ -3949,7 +3952,7 @@
         <v>1</v>
       </c>
       <c r="F87" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G87" s="37" t="s">
         <v>1</v>
@@ -3972,7 +3975,7 @@
         <v>1</v>
       </c>
       <c r="F88" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G88" s="37" t="s">
         <v>1</v>
@@ -3995,7 +3998,7 @@
         <v>1</v>
       </c>
       <c r="F89" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G89" s="37" t="s">
         <v>1</v>
@@ -4018,7 +4021,7 @@
         <v>1</v>
       </c>
       <c r="F90" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G90" s="37" t="s">
         <v>1</v>
@@ -4041,7 +4044,7 @@
         <v>1</v>
       </c>
       <c r="F91" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G91" s="37" t="s">
         <v>1</v>
@@ -4064,7 +4067,7 @@
         <v>1</v>
       </c>
       <c r="F92" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G92" s="37" t="s">
         <v>1</v>
@@ -4087,7 +4090,7 @@
         <v>1</v>
       </c>
       <c r="F93" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G93" s="37" t="s">
         <v>1</v>
@@ -4110,7 +4113,7 @@
         <v>1</v>
       </c>
       <c r="F94" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G94" s="37" t="s">
         <v>1</v>
@@ -4133,7 +4136,7 @@
         <v>1</v>
       </c>
       <c r="F95" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G95" s="37" t="s">
         <v>1</v>
@@ -4156,7 +4159,7 @@
         <v>1</v>
       </c>
       <c r="F96" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G96" s="37" t="s">
         <v>1</v>
@@ -4179,7 +4182,7 @@
         <v>1</v>
       </c>
       <c r="F97" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G97" s="37" t="s">
         <v>1</v>
@@ -4202,7 +4205,7 @@
         <v>1</v>
       </c>
       <c r="F98" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G98" s="37" t="s">
         <v>1</v>
@@ -4225,7 +4228,7 @@
         <v>1</v>
       </c>
       <c r="F99" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G99" s="37" t="s">
         <v>1</v>
@@ -4248,7 +4251,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G100" s="37" t="s">
         <v>1</v>
@@ -4266,41 +4269,41 @@
   <dimension ref="B1:K15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:H2"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="3" customWidth="1"/>
     <col min="2" max="3" width="4.140625" style="3" customWidth="1"/>
-    <col min="4" max="11" width="18" style="3" customWidth="1"/>
+    <col min="4" max="11" width="17.7109375" style="3" customWidth="1"/>
     <col min="12" max="12" width="1" style="3" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="48" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="50" t="s">
-        <v>214</v>
-      </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="50" t="s">
+      <c r="E2" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="40"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="49"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="4" t="s">
         <v>137</v>
       </c>
@@ -4324,10 +4327,10 @@
       </c>
     </row>
     <row r="4" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="44" t="s">
         <v>145</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -4356,8 +4359,8 @@
       </c>
     </row>
     <row r="5" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="42"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="14" t="s">
         <v>154</v>
       </c>
@@ -4384,8 +4387,8 @@
       </c>
     </row>
     <row r="6" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
-      <c r="C6" s="42" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="45" t="s">
         <v>161</v>
       </c>
       <c r="D6" s="20" t="s">
@@ -4414,8 +4417,8 @@
       </c>
     </row>
     <row r="7" spans="2:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="40"/>
-      <c r="C7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="23" t="s">
         <v>168</v>
       </c>
@@ -4442,10 +4445,10 @@
       </c>
     </row>
     <row r="8" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="48" t="s">
         <v>176</v>
       </c>
       <c r="D8" s="29" t="s">
@@ -4464,151 +4467,151 @@
         <v>178</v>
       </c>
       <c r="I8" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="K8" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="J8" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="K8" s="35" t="s">
+    </row>
+    <row r="9" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="42"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="14" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="39"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="14" t="s">
+      <c r="E9" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="F9" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="K9" s="19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="42"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="K9" s="19" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="14" t="s">
+      <c r="E10" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>186</v>
-      </c>
       <c r="F10" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>187</v>
+        <v>213</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
       <c r="K10" s="22" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="39"/>
-      <c r="C11" s="42" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="G11" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="H11" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="I11" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="J11" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="K11" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="I11" s="1" t="s">
+    </row>
+    <row r="12" spans="2:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="43"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="E12" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="F12" s="25" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="40"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="23" t="s">
+      <c r="G12" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="H12" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="I12" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="J12" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="K12" s="28" t="s">
         <v>202</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="J12" s="27" t="s">
-        <v>204</v>
-      </c>
-      <c r="K12" s="28" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D14" s="36" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" r:id="rId1"/>

</xml_diff>